<commit_message>
feature: new events added to timeline
</commit_message>
<xml_diff>
--- a/input/Etkinlik Takvimi.xlsx
+++ b/input/Etkinlik Takvimi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>İsim</t>
   </si>
@@ -73,7 +73,19 @@
     <t>Yapay Zeka Kulübü</t>
   </si>
   <si>
-    <t>21.09.2022</t>
+    <t>Mobidictum Konferansı</t>
+  </si>
+  <si>
+    <t>07.09.2022</t>
+  </si>
+  <si>
+    <t>18.09.2022</t>
+  </si>
+  <si>
+    <t>Unity Eğitimi</t>
+  </si>
+  <si>
+    <t>25.09.2022</t>
   </si>
   <si>
     <t>1. Kaggle Yarışması</t>
@@ -82,18 +94,36 @@
     <t>30.09.2022</t>
   </si>
   <si>
+    <t>Bilişim Suçları Konferansı</t>
+  </si>
+  <si>
+    <t>01.10.2022</t>
+  </si>
+  <si>
     <t>2. GameJam</t>
   </si>
   <si>
     <t>08.10.2022</t>
   </si>
   <si>
-    <t>Machine Learning Workshopu</t>
+    <t>Eurasia Blockchain Zirvesi</t>
+  </si>
+  <si>
+    <t>09.10.2022</t>
+  </si>
+  <si>
+    <t>Makine Öğrenmesi Eğitimi</t>
   </si>
   <si>
     <t>10.10.2022</t>
   </si>
   <si>
+    <t>Sürdürülebilir Web3 Zirvesi</t>
+  </si>
+  <si>
+    <t>24.10.2022</t>
+  </si>
+  <si>
     <t>2. Kaggle Yarışması</t>
   </si>
   <si>
@@ -110,6 +140,105 @@
   </si>
   <si>
     <t>13.11.2022</t>
+  </si>
+  <si>
+    <t>OBSS Üniversiteler Buluşması</t>
+  </si>
+  <si>
+    <t>07.12.2022</t>
+  </si>
+  <si>
+    <t>Devletler için Blockchain Webinarı</t>
+  </si>
+  <si>
+    <t>26.12.2022</t>
+  </si>
+  <si>
+    <t>Maharishi Üniversitesi Tanıtımı</t>
+  </si>
+  <si>
+    <t>12.01.2023</t>
+  </si>
+  <si>
+    <t>Minecraft Serverı Kuruluşu</t>
+  </si>
+  <si>
+    <t>19.01.2023</t>
+  </si>
+  <si>
+    <t>Oyunla Gelecek Söyleşisi</t>
+  </si>
+  <si>
+    <t>24.01.2023</t>
+  </si>
+  <si>
+    <t>Hesaplamalı Hukuk Konferansı</t>
+  </si>
+  <si>
+    <t>28.01.2023</t>
+  </si>
+  <si>
+    <t>Blockchain ve Güvenlik Webinarı</t>
+  </si>
+  <si>
+    <t>27.01.2023</t>
+  </si>
+  <si>
+    <t>1. Mezun Söyleşisi</t>
+  </si>
+  <si>
+    <t>04.02.2023</t>
+  </si>
+  <si>
+    <t>PostgreSQL Eğitimi</t>
+  </si>
+  <si>
+    <t>05.02.2023</t>
+  </si>
+  <si>
+    <t>Binance ve Üniversiteler Söyleşisi</t>
+  </si>
+  <si>
+    <t>15.03.2023</t>
+  </si>
+  <si>
+    <t>2. Mezun Söyleşisi</t>
+  </si>
+  <si>
+    <t>12.04.2023</t>
+  </si>
+  <si>
+    <t>Girişimcilik Dünyası Webinarı</t>
+  </si>
+  <si>
+    <t>14.04.2023</t>
+  </si>
+  <si>
+    <t>Uygulama Geliştirme Kulübü</t>
+  </si>
+  <si>
+    <t>Riot Games Webinarı</t>
+  </si>
+  <si>
+    <t>15.04.2023</t>
+  </si>
+  <si>
+    <t>CerebrumTech Webinarı</t>
+  </si>
+  <si>
+    <t>18.04.2023</t>
+  </si>
+  <si>
+    <t>3. Mezun Söyleşisi</t>
+  </si>
+  <si>
+    <t>29.04.2023</t>
+  </si>
+  <si>
+    <t>2. Ceket Sohbeti</t>
+  </si>
+  <si>
+    <t>22.05.2023</t>
   </si>
 </sst>
 </file>
@@ -117,9 +246,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -139,6 +268,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -147,17 +333,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -171,113 +406,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,187 +421,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,25 +625,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +680,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -568,166 +712,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1054,18 +1183,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="25.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="31.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="10.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="12.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="20.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1172,36 +1301,36 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>0.625</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="D7" s="2">
-        <v>0.708333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="D8" s="2">
-        <v>0.916666666666667</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1212,10 +1341,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="2">
-        <v>0.5</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D9" s="2">
-        <v>0.916666666666667</v>
+        <v>0.6875</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1229,7 +1358,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="2">
-        <v>0.833333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="2">
         <v>0.916666666666667</v>
@@ -1246,13 +1375,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="2">
-        <v>0.5</v>
+        <v>0.604166666666667</v>
       </c>
       <c r="D11" s="2">
-        <v>0.916666666666667</v>
+        <v>0.708333333333333</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1263,13 +1392,13 @@
         <v>29</v>
       </c>
       <c r="C12" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="2">
         <v>0.916666666666667</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1280,13 +1409,370 @@
         <v>31</v>
       </c>
       <c r="C13" s="2">
-        <v>0.5</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="D13" s="2">
-        <v>0.916666666666667</v>
+        <v>0.75</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.854166666666667</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.770833333333333</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: group and hour data added vis js timeline
</commit_message>
<xml_diff>
--- a/input/Etkinlik Takvimi.xlsx
+++ b/input/Etkinlik Takvimi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>İsim</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Düzenleyen</t>
+  </si>
+  <si>
+    <t>Detaylı Açıklama</t>
   </si>
   <si>
     <t>Kuruluş Toplantısı</t>
@@ -247,9 +250,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -269,7 +272,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,15 +300,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,28 +324,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -342,23 +333,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -388,17 +371,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,6 +385,35 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -421,187 +424,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,26 +618,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,16 +682,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,18 +706,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,130 +736,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1183,21 +1186,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="31.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="10.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="12.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="18.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,13 +1217,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>0.833333333333333</v>
@@ -1228,15 +1235,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>0.583333333333333</v>
@@ -1245,15 +1252,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>0.625</v>
@@ -1262,15 +1269,15 @@
         <v>0.75</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2">
         <v>0.5</v>
@@ -1279,15 +1286,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>0.75</v>
@@ -1296,15 +1303,15 @@
         <v>0.833333333333333</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <v>0.416666666666667</v>
@@ -1313,15 +1320,15 @@
         <v>0.75</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
         <v>0.625</v>
@@ -1330,15 +1337,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2">
         <v>0.604166666666667</v>
@@ -1347,15 +1354,15 @@
         <v>0.6875</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
         <v>0.5</v>
@@ -1364,15 +1371,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
         <v>0.604166666666667</v>
@@ -1381,15 +1388,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>0.5</v>
@@ -1398,15 +1405,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>0.416666666666667</v>
@@ -1415,15 +1422,15 @@
         <v>0.75</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2">
         <v>0.833333333333333</v>
@@ -1432,15 +1439,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2">
         <v>0.416666666666667</v>
@@ -1449,15 +1456,15 @@
         <v>0.625</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2">
         <v>0.5</v>
@@ -1466,15 +1473,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2">
         <v>0.75</v>
@@ -1483,15 +1490,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>0.5</v>
@@ -1500,15 +1507,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2">
         <v>0.666666666666667</v>
@@ -1517,15 +1524,15 @@
         <v>0.75</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2">
         <v>0.833333333333333</v>
@@ -1534,15 +1541,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2">
         <v>0.666666666666667</v>
@@ -1551,15 +1558,15 @@
         <v>0.75</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2">
         <v>0.5</v>
@@ -1568,15 +1575,15 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2">
         <v>0.625</v>
@@ -1585,15 +1592,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2">
         <v>0.666666666666667</v>
@@ -1602,15 +1609,15 @@
         <v>0.75</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2">
         <v>0.833333333333333</v>
@@ -1619,15 +1626,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2">
         <v>0.875</v>
@@ -1636,15 +1643,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2">
         <v>0.6875</v>
@@ -1653,15 +1660,15 @@
         <v>0.8125</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2">
         <v>0.833333333333333</v>
@@ -1670,15 +1677,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2">
         <v>0.729166666666667</v>
@@ -1687,15 +1694,15 @@
         <v>0.75</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2">
         <v>0.875</v>
@@ -1704,15 +1711,15 @@
         <v>0.9375</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31" s="2">
         <v>0.833333333333333</v>
@@ -1721,15 +1728,15 @@
         <v>0.875</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2">
         <v>0.8125</v>
@@ -1738,15 +1745,15 @@
         <v>0.854166666666667</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" s="2">
         <v>0.770833333333333</v>
@@ -1755,15 +1762,15 @@
         <v>0.791666666666667</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" s="2">
         <v>0.791666666666667</v>
@@ -1772,7 +1779,7 @@
         <v>0.958333333333333</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: title added for club names
</commit_message>
<xml_diff>
--- a/input/Etkinlik Takvimi.xlsx
+++ b/input/Etkinlik Takvimi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>İsim</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Düzenleyen</t>
-  </si>
-  <si>
-    <t>Detaylı Açıklama</t>
   </si>
   <si>
     <t>Kuruluş Toplantısı</t>
@@ -249,8 +246,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -271,8 +268,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,20 +284,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -308,9 +292,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,48 +368,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,6 +378,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,29 +406,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -424,13 +421,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,25 +577,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,139 +589,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,6 +641,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,19 +712,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -736,130 +733,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1189,7 +1186,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1217,16 +1214,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>0.833333333333333</v>
@@ -1235,15 +1230,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>0.583333333333333</v>
@@ -1252,15 +1247,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>0.625</v>
@@ -1269,15 +1264,15 @@
         <v>0.75</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="2">
         <v>0.5</v>
@@ -1286,15 +1281,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>0.75</v>
@@ -1303,15 +1298,15 @@
         <v>0.833333333333333</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="2">
         <v>0.416666666666667</v>
@@ -1320,15 +1315,15 @@
         <v>0.75</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>0.625</v>
@@ -1337,15 +1332,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="2">
         <v>0.604166666666667</v>
@@ -1354,15 +1349,15 @@
         <v>0.6875</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="2">
         <v>0.5</v>
@@ -1371,15 +1366,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="2">
         <v>0.604166666666667</v>
@@ -1388,15 +1383,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>0.5</v>
@@ -1405,15 +1400,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>0.416666666666667</v>
@@ -1422,15 +1417,15 @@
         <v>0.75</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="2">
         <v>0.833333333333333</v>
@@ -1439,15 +1434,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="2">
         <v>0.416666666666667</v>
@@ -1456,15 +1451,15 @@
         <v>0.625</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="2">
         <v>0.5</v>
@@ -1473,15 +1468,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
       </c>
       <c r="C17" s="2">
         <v>0.75</v>
@@ -1490,15 +1485,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
         <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>0.5</v>
@@ -1507,15 +1502,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
         <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
       </c>
       <c r="C19" s="2">
         <v>0.666666666666667</v>
@@ -1524,15 +1519,15 @@
         <v>0.75</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
       </c>
       <c r="C20" s="2">
         <v>0.833333333333333</v>
@@ -1541,15 +1536,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
       </c>
       <c r="C21" s="2">
         <v>0.666666666666667</v>
@@ -1558,15 +1553,15 @@
         <v>0.75</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>50</v>
       </c>
       <c r="C22" s="2">
         <v>0.5</v>
@@ -1575,15 +1570,15 @@
         <v>0.541666666666667</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
       </c>
       <c r="C23" s="2">
         <v>0.625</v>
@@ -1592,15 +1587,15 @@
         <v>0.708333333333333</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
       </c>
       <c r="C24" s="2">
         <v>0.666666666666667</v>
@@ -1609,15 +1604,15 @@
         <v>0.75</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
       </c>
       <c r="C25" s="2">
         <v>0.833333333333333</v>
@@ -1626,15 +1621,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
       </c>
       <c r="C26" s="2">
         <v>0.875</v>
@@ -1643,15 +1638,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
       </c>
       <c r="C27" s="2">
         <v>0.6875</v>
@@ -1660,15 +1655,15 @@
         <v>0.8125</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
       </c>
       <c r="C28" s="2">
         <v>0.833333333333333</v>
@@ -1677,15 +1672,15 @@
         <v>0.916666666666667</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
       </c>
       <c r="C29" s="2">
         <v>0.729166666666667</v>
@@ -1694,15 +1689,15 @@
         <v>0.75</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
         <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
       </c>
       <c r="C30" s="2">
         <v>0.875</v>
@@ -1711,15 +1706,15 @@
         <v>0.9375</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" t="s">
-        <v>69</v>
       </c>
       <c r="C31" s="2">
         <v>0.833333333333333</v>
@@ -1728,15 +1723,15 @@
         <v>0.875</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
         <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>71</v>
       </c>
       <c r="C32" s="2">
         <v>0.8125</v>
@@ -1745,15 +1740,15 @@
         <v>0.854166666666667</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" t="s">
-        <v>73</v>
       </c>
       <c r="C33" s="2">
         <v>0.770833333333333</v>
@@ -1762,15 +1757,15 @@
         <v>0.791666666666667</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
         <v>74</v>
-      </c>
-      <c r="B34" t="s">
-        <v>75</v>
       </c>
       <c r="C34" s="2">
         <v>0.791666666666667</v>
@@ -1779,7 +1774,7 @@
         <v>0.958333333333333</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>